<commit_message>
added web: bestcheque, booking
</commit_message>
<xml_diff>
--- a/working_windows_extension/version_4/member web/bestcheque/Expenses.xlsx
+++ b/working_windows_extension/version_4/member web/bestcheque/Expenses.xlsx
@@ -14,42 +14,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
-  <si>
-    <t>Confirmation Number</t>
-  </si>
-  <si>
-    <t>CRS Number</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Booking.com Price</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+  <si>
+    <t>Conf number</t>
+  </si>
+  <si>
+    <t>Guest Name</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>227249103-01</t>
   </si>
   <si>
     <t>YRIS HERNANDEZ</t>
   </si>
   <si>
-    <t>Checked in, but different date</t>
+    <t>Date changed</t>
   </si>
   <si>
     <t>480526504-01</t>
   </si>
   <si>
     <t>KAVITA CHALLA</t>
-  </si>
-  <si>
-    <t>:1</t>
   </si>
   <si>
     <t>RUIYING DING</t>
@@ -387,13 +378,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -406,59 +397,47 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>97.58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>400.16</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>97.58</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>17002077715</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4">
+        <v>130.38</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
-      </c>
-      <c r="D3">
-        <v>400.16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>17002077715</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>130.38</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>